<commit_message>
Adding in 1-many on actions for a snapshot. Cleaned up UI for dashboard.
</commit_message>
<xml_diff>
--- a/lib/SEMAT_Alpha_Cards_CMU_1.1.xlsx
+++ b/lib/SEMAT_Alpha_Cards_CMU_1.1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="218">
   <si>
     <t>Stakeholders</t>
   </si>
@@ -231,12 +231,6 @@
     <t>Stakeholders confirm that system meets their expectations.</t>
   </si>
   <si>
-    <t>Providing Feedback</t>
-  </si>
-  <si>
-    <t>Stakeholders provide feedback on their experiences</t>
-  </si>
-  <si>
     <t>Software can solve the problem.</t>
   </si>
   <si>
@@ -255,9 +249,6 @@
     <t>Stakeholder representatives are appointed</t>
   </si>
   <si>
-    <t>Stakeholder representatives agreed to take on responsibilities</t>
-  </si>
-  <si>
     <t>Stakeholders agree on collaboration approach</t>
   </si>
   <si>
@@ -291,9 +282,6 @@
     <t>Software-based solution addresses an identified opportunity</t>
   </si>
   <si>
-    <t>A stakeholder wishes to make an investment in better understanding potential value</t>
-  </si>
-  <si>
     <t>Problem is clearly articulated</t>
   </si>
   <si>
@@ -342,9 +330,6 @@
     <t>Purpose and extent of system are agreed</t>
   </si>
   <si>
-    <t>Scope constraints and assumptions are identified</t>
-  </si>
-  <si>
     <t>Processes and tools for handling requirements are in place</t>
   </si>
   <si>
@@ -357,9 +342,6 @@
     <t>Requirements are prioritized</t>
   </si>
   <si>
-    <t>Requirements make sense relative to each other</t>
-  </si>
-  <si>
     <t>Rationale and impact are understood</t>
   </si>
   <si>
@@ -405,18 +387,9 @@
     <t>Relevant stakeholders agree architecture is appropriate</t>
   </si>
   <si>
-    <t>Critical interfaces and system configurations tested</t>
-  </si>
-  <si>
     <t>Users can operate system</t>
   </si>
   <si>
-    <t>System has desired quality characteristics</t>
-  </si>
-  <si>
-    <t>Functionality and performance are tested and accepted</t>
-  </si>
-  <si>
     <t>Defect levels are acceptable</t>
   </si>
   <si>
@@ -468,9 +441,6 @@
     <t>Decision making processes are decided</t>
   </si>
   <si>
-    <t>Team has enough resources to address opportunity</t>
-  </si>
-  <si>
     <t>Team organization, responsibilities, and roles are understood</t>
   </si>
   <si>
@@ -510,24 +480,9 @@
     <t>Team is no longer accountable</t>
   </si>
   <si>
-    <t>Principles and Values Established</t>
-  </si>
-  <si>
-    <t>Principles and values are established</t>
-  </si>
-  <si>
-    <t>Team commits to principles and values</t>
-  </si>
-  <si>
-    <t>Stakeholders accept team's principles and values</t>
-  </si>
-  <si>
     <t>Practices and tools are identified to address team's needs</t>
   </si>
   <si>
-    <t>Practices and tools are consistent with principles &amp; values</t>
-  </si>
-  <si>
     <t>A transition plan is defined to adopt new practices and tools</t>
   </si>
   <si>
@@ -666,7 +621,58 @@
     <t>Unplanned work is manageable</t>
   </si>
   <si>
-    <t>Representatives respect team's principles</t>
+    <t>Experimenting</t>
+  </si>
+  <si>
+    <t>Stakeholders provide feedback on their experiences with the deployed system</t>
+  </si>
+  <si>
+    <t>Stakeholder representatives agree to take on responsibilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Representatives respect team's way of working </t>
+  </si>
+  <si>
+    <t>Stakeholders wish to make an investment in better understanding potential value</t>
+  </si>
+  <si>
+    <t>Assumptions made while defining requirements are captured</t>
+  </si>
+  <si>
+    <t>Scope constraints are identified</t>
+  </si>
+  <si>
+    <t>There are no conflicting requirements</t>
+  </si>
+  <si>
+    <t>Critical interfaces and system configurations demonstrated</t>
+  </si>
+  <si>
+    <t>System has desired quality and performance characteristics</t>
+  </si>
+  <si>
+    <t>Functionality is tested and accepted</t>
+  </si>
+  <si>
+    <t>Team has enough resources to start addressing opportunity</t>
+  </si>
+  <si>
+    <t>Values and Principles Established</t>
+  </si>
+  <si>
+    <t>Values and principles are identified</t>
+  </si>
+  <si>
+    <t>Team commits to values and principles</t>
+  </si>
+  <si>
+    <t>Stakeholders accept team's values and principles</t>
+  </si>
+  <si>
+    <t>Practices and tools are consistent with values and principles</t>
+  </si>
+  <si>
+    <t>Constraints about practices and tools are known</t>
   </si>
 </sst>
 </file>
@@ -803,8 +809,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="105">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -969,7 +995,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="105">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1022,6 +1048,16 @@
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1074,6 +1110,16 @@
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1459,11 +1505,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U288"/>
+  <dimension ref="A1:U289"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G216" sqref="G216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1599,7 +1645,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1624,7 +1670,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1649,7 +1695,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1699,7 +1745,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1724,7 +1770,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="17" t="s">
-        <v>78</v>
+        <v>202</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1749,7 +1795,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1774,7 +1820,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="17" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1799,7 +1845,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1849,7 +1895,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1874,7 +1920,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1899,7 +1945,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1949,7 +1995,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1974,7 +2020,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1999,7 +2045,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -2024,7 +2070,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -2120,7 +2166,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -2167,7 +2213,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="2"/>
@@ -2193,7 +2239,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2" t="s">
-        <v>71</v>
+        <v>201</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -2395,7 +2441,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -2420,7 +2466,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
-        <v>90</v>
+        <v>204</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -2493,7 +2539,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -2518,7 +2564,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -2543,7 +2589,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -2639,7 +2685,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -2664,7 +2710,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -2689,7 +2735,7 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -2714,7 +2760,7 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
@@ -2787,7 +2833,7 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -2812,7 +2858,7 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -2837,7 +2883,7 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -2956,7 +3002,7 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
@@ -2981,7 +3027,7 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -3006,7 +3052,7 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -3079,7 +3125,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -3104,7 +3150,7 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -3210,7 +3256,7 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="18" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -3235,7 +3281,7 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="18" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
@@ -3331,7 +3377,7 @@
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
@@ -3356,7 +3402,7 @@
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -3381,7 +3427,7 @@
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -3406,7 +3452,7 @@
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="18" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -3430,7 +3476,9 @@
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
-      <c r="G79" s="18"/>
+      <c r="G79" s="18" t="s">
+        <v>205</v>
+      </c>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
@@ -3571,7 +3619,7 @@
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
@@ -3596,7 +3644,7 @@
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="18" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
@@ -3621,7 +3669,7 @@
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="18" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
@@ -3646,7 +3694,7 @@
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="18" t="s">
-        <v>112</v>
+        <v>207</v>
       </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -3671,7 +3719,7 @@
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="18" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
@@ -3813,7 +3861,7 @@
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="18" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
@@ -3838,7 +3886,7 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="18" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
@@ -3863,7 +3911,7 @@
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="18" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
@@ -3888,7 +3936,7 @@
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="18" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
@@ -3961,7 +4009,7 @@
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
       <c r="G101" s="18" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
@@ -3986,7 +4034,7 @@
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="18" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
@@ -4082,7 +4130,7 @@
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
       <c r="G106" s="18" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
@@ -4107,7 +4155,7 @@
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
       <c r="G107" s="18" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
@@ -4132,7 +4180,7 @@
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
       <c r="G108" s="18" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
@@ -4237,7 +4285,7 @@
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="18" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
@@ -4262,7 +4310,7 @@
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="18" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
@@ -4287,7 +4335,7 @@
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="18" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
@@ -4312,7 +4360,7 @@
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
@@ -4337,7 +4385,7 @@
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="18" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
@@ -4362,7 +4410,7 @@
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
       <c r="G117" s="18" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
@@ -4435,7 +4483,7 @@
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
@@ -4460,7 +4508,7 @@
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="18" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
@@ -4485,7 +4533,7 @@
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="18" t="s">
-        <v>128</v>
+        <v>208</v>
       </c>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
@@ -4604,7 +4652,7 @@
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
       <c r="G127" s="18" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
@@ -4629,7 +4677,7 @@
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="18" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
@@ -4654,7 +4702,7 @@
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="18" t="s">
-        <v>131</v>
+        <v>210</v>
       </c>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
@@ -4679,7 +4727,7 @@
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
       <c r="G130" s="18" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
@@ -4821,7 +4869,7 @@
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
       <c r="G136" s="18" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="H136" s="2"/>
       <c r="I136" s="2"/>
@@ -4846,7 +4894,7 @@
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
       <c r="G137" s="18" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
@@ -4942,7 +4990,7 @@
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
       <c r="G141" s="18" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="H141" s="2"/>
       <c r="I141" s="2"/>
@@ -4967,7 +5015,7 @@
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
       <c r="G142" s="18" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H142" s="2"/>
       <c r="I142" s="2"/>
@@ -4992,7 +5040,7 @@
       <c r="E143" s="2"/>
       <c r="F143" s="2"/>
       <c r="G143" s="2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H143" s="2"/>
       <c r="I143" s="2"/>
@@ -5039,7 +5087,7 @@
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
       <c r="F145" s="2" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="G145" s="6"/>
       <c r="H145" s="2"/>
@@ -5065,7 +5113,7 @@
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="H146" s="2"/>
       <c r="I146" s="2"/>
@@ -5090,7 +5138,7 @@
       <c r="E147" s="2"/>
       <c r="F147" s="2"/>
       <c r="G147" s="2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="H147" s="2"/>
       <c r="I147" s="2"/>
@@ -5115,7 +5163,7 @@
       <c r="E148" s="2"/>
       <c r="F148" s="2"/>
       <c r="G148" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="H148" s="2"/>
       <c r="I148" s="2"/>
@@ -5140,7 +5188,7 @@
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="H149" s="2"/>
       <c r="I149" s="2"/>
@@ -5165,7 +5213,7 @@
       <c r="E150" s="2"/>
       <c r="F150" s="2"/>
       <c r="G150" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="H150" s="2"/>
       <c r="I150" s="2"/>
@@ -5237,7 +5285,7 @@
       <c r="E153" s="2"/>
       <c r="F153" s="2"/>
       <c r="G153" s="18" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="H153" s="2"/>
       <c r="I153" s="2"/>
@@ -5411,7 +5459,7 @@
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
       <c r="G160" s="18" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="H160" s="2"/>
       <c r="I160" s="2"/>
@@ -5436,7 +5484,7 @@
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
       <c r="G161" s="18" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="H161" s="2"/>
       <c r="I161" s="2"/>
@@ -5461,7 +5509,7 @@
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
       <c r="G162" s="18" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
@@ -5486,7 +5534,7 @@
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
       <c r="G163" s="18" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="H163" s="2"/>
       <c r="I163" s="2"/>
@@ -5511,7 +5559,7 @@
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="18" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="H164" s="2"/>
       <c r="I164" s="2"/>
@@ -5536,7 +5584,7 @@
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
       <c r="G165" s="18" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="H165" s="2"/>
       <c r="I165" s="2"/>
@@ -5561,7 +5609,7 @@
       <c r="E166" s="2"/>
       <c r="F166" s="2"/>
       <c r="G166" s="18" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="H166" s="2"/>
       <c r="I166" s="2"/>
@@ -5703,7 +5751,7 @@
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
       <c r="G172" s="18" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="H172" s="2"/>
       <c r="I172" s="2"/>
@@ -5728,7 +5776,7 @@
       <c r="E173" s="2"/>
       <c r="F173" s="2"/>
       <c r="G173" s="18" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="H173" s="2"/>
       <c r="I173" s="2"/>
@@ -5753,7 +5801,7 @@
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
       <c r="G174" s="18" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="H174" s="2"/>
       <c r="I174" s="2"/>
@@ -5778,7 +5826,7 @@
       <c r="E175" s="2"/>
       <c r="F175" s="2"/>
       <c r="G175" s="18" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="H175" s="2"/>
       <c r="I175" s="2"/>
@@ -5966,7 +6014,7 @@
       <c r="E183" s="2"/>
       <c r="F183" s="2"/>
       <c r="G183" s="18" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
@@ -5991,7 +6039,7 @@
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
       <c r="G184" s="18" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="H184" s="2"/>
       <c r="I184" s="2"/>
@@ -6016,7 +6064,7 @@
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
       <c r="G185" s="18" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="H185" s="2"/>
       <c r="I185" s="2"/>
@@ -6041,7 +6089,7 @@
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
       <c r="G186" s="18" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="H186" s="2"/>
       <c r="I186" s="2"/>
@@ -6114,7 +6162,7 @@
       <c r="E189" s="2"/>
       <c r="F189" s="2"/>
       <c r="G189" s="18" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="H189" s="2"/>
       <c r="I189" s="2"/>
@@ -6139,7 +6187,7 @@
       <c r="E190" s="2"/>
       <c r="F190" s="2"/>
       <c r="G190" s="18" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="H190" s="2"/>
       <c r="I190" s="2"/>
@@ -6158,7 +6206,7 @@
     </row>
     <row r="191" spans="1:21" ht="12">
       <c r="G191" s="18" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="192" spans="1:21" ht="12">
@@ -6169,7 +6217,7 @@
       <c r="E192" s="2"/>
       <c r="F192" s="2"/>
       <c r="G192" s="2" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="H192" s="2"/>
       <c r="I192" s="2"/>
@@ -6194,7 +6242,7 @@
       <c r="E193" s="2"/>
       <c r="F193" s="2"/>
       <c r="G193" s="18" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="H193" s="2"/>
       <c r="I193" s="2"/>
@@ -6313,7 +6361,7 @@
       <c r="E198" s="2"/>
       <c r="F198" s="2"/>
       <c r="G198" s="18" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="H198" s="2"/>
       <c r="I198" s="2"/>
@@ -6449,14 +6497,14 @@
       <c r="T203" s="2"/>
       <c r="U203" s="2"/>
     </row>
-    <row r="204" spans="1:21" ht="24">
+    <row r="204" spans="1:21" ht="36">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
       <c r="F204" s="15" t="s">
-        <v>163</v>
+        <v>212</v>
       </c>
       <c r="G204" s="10"/>
       <c r="H204" s="2"/>
@@ -6482,7 +6530,7 @@
       <c r="E205" s="2"/>
       <c r="F205" s="2"/>
       <c r="G205" s="18" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="H205" s="2"/>
       <c r="I205" s="2"/>
@@ -6507,7 +6555,7 @@
       <c r="E206" s="2"/>
       <c r="F206" s="2"/>
       <c r="G206" s="18" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="H206" s="2"/>
       <c r="I206" s="2"/>
@@ -6532,7 +6580,7 @@
       <c r="E207" s="2"/>
       <c r="F207" s="2"/>
       <c r="G207" s="18" t="s">
-        <v>166</v>
+        <v>215</v>
       </c>
       <c r="H207" s="2"/>
       <c r="I207" s="2"/>
@@ -6671,7 +6719,7 @@
       <c r="D213" s="2"/>
       <c r="E213" s="2"/>
       <c r="F213" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="G213" s="10"/>
       <c r="H213" s="2"/>
@@ -6697,7 +6745,7 @@
       <c r="E214" s="2"/>
       <c r="F214" s="2"/>
       <c r="G214" s="18" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="H214" s="2"/>
       <c r="I214" s="2"/>
@@ -6714,7 +6762,7 @@
       <c r="T214" s="2"/>
       <c r="U214" s="2"/>
     </row>
-    <row r="215" spans="1:21" ht="12">
+    <row r="215" spans="1:21" s="9" customFormat="1" ht="12">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
@@ -6722,7 +6770,7 @@
       <c r="E215" s="2"/>
       <c r="F215" s="2"/>
       <c r="G215" s="18" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="H215" s="2"/>
       <c r="I215" s="2"/>
@@ -6747,7 +6795,7 @@
       <c r="E216" s="2"/>
       <c r="F216" s="2"/>
       <c r="G216" s="18" t="s">
-        <v>169</v>
+        <v>216</v>
       </c>
       <c r="H216" s="2"/>
       <c r="I216" s="2"/>
@@ -6772,7 +6820,7 @@
       <c r="E217" s="2"/>
       <c r="F217" s="2"/>
       <c r="G217" s="18" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="H217" s="2"/>
       <c r="I217" s="2"/>
@@ -6796,7 +6844,9 @@
       <c r="D218" s="2"/>
       <c r="E218" s="2"/>
       <c r="F218" s="2"/>
-      <c r="G218" s="18"/>
+      <c r="G218" s="18" t="s">
+        <v>155</v>
+      </c>
       <c r="H218" s="2"/>
       <c r="I218" s="2"/>
       <c r="J218" s="2"/>
@@ -6842,7 +6892,7 @@
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
       <c r="F220" s="2"/>
-      <c r="G220" s="12"/>
+      <c r="G220" s="18"/>
       <c r="H220" s="2"/>
       <c r="I220" s="2"/>
       <c r="J220" s="2"/>
@@ -6864,10 +6914,8 @@
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
-      <c r="F221" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G221" s="10"/>
+      <c r="F221" s="2"/>
+      <c r="G221" s="12"/>
       <c r="H221" s="2"/>
       <c r="I221" s="2"/>
       <c r="J221" s="2"/>
@@ -6889,10 +6937,10 @@
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
       <c r="E222" s="2"/>
-      <c r="F222" s="2"/>
-      <c r="G222" s="18" t="s">
-        <v>171</v>
-      </c>
+      <c r="F222" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G222" s="10"/>
       <c r="H222" s="2"/>
       <c r="I222" s="2"/>
       <c r="J222" s="2"/>
@@ -6916,7 +6964,7 @@
       <c r="E223" s="2"/>
       <c r="F223" s="2"/>
       <c r="G223" s="18" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="H223" s="2"/>
       <c r="I223" s="2"/>
@@ -6941,7 +6989,7 @@
       <c r="E224" s="2"/>
       <c r="F224" s="2"/>
       <c r="G224" s="18" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="H224" s="2"/>
       <c r="I224" s="2"/>
@@ -6966,7 +7014,7 @@
       <c r="E225" s="2"/>
       <c r="F225" s="2"/>
       <c r="G225" s="18" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="H225" s="2"/>
       <c r="I225" s="2"/>
@@ -6990,7 +7038,9 @@
       <c r="D226" s="2"/>
       <c r="E226" s="2"/>
       <c r="F226" s="2"/>
-      <c r="G226" s="18"/>
+      <c r="G226" s="18" t="s">
+        <v>159</v>
+      </c>
       <c r="H226" s="2"/>
       <c r="I226" s="2"/>
       <c r="J226" s="2"/>
@@ -7006,7 +7056,7 @@
       <c r="T226" s="2"/>
       <c r="U226" s="2"/>
     </row>
-    <row r="227" spans="1:21" s="9" customFormat="1" ht="12">
+    <row r="227" spans="1:21" ht="12">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
@@ -7029,14 +7079,14 @@
       <c r="T227" s="2"/>
       <c r="U227" s="2"/>
     </row>
-    <row r="228" spans="1:21" ht="12">
+    <row r="228" spans="1:21" s="9" customFormat="1" ht="12">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
-      <c r="F228" s="16"/>
-      <c r="G228" s="10"/>
+      <c r="F228" s="2"/>
+      <c r="G228" s="18"/>
       <c r="H228" s="2"/>
       <c r="I228" s="2"/>
       <c r="J228" s="2"/>
@@ -7058,8 +7108,8 @@
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
       <c r="E229" s="2"/>
-      <c r="F229" s="2"/>
-      <c r="G229" s="18"/>
+      <c r="F229" s="16"/>
+      <c r="G229" s="10"/>
       <c r="H229" s="2"/>
       <c r="I229" s="2"/>
       <c r="J229" s="2"/>
@@ -7127,10 +7177,8 @@
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
       <c r="E232" s="2"/>
-      <c r="F232" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G232" s="10"/>
+      <c r="F232" s="2"/>
+      <c r="G232" s="18"/>
       <c r="H232" s="2"/>
       <c r="I232" s="2"/>
       <c r="J232" s="2"/>
@@ -7152,10 +7200,10 @@
       <c r="C233" s="2"/>
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
-      <c r="F233" s="2"/>
-      <c r="G233" s="18" t="s">
-        <v>175</v>
-      </c>
+      <c r="F233" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G233" s="10"/>
       <c r="H233" s="2"/>
       <c r="I233" s="2"/>
       <c r="J233" s="2"/>
@@ -7179,7 +7227,7 @@
       <c r="E234" s="2"/>
       <c r="F234" s="2"/>
       <c r="G234" s="18" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="H234" s="2"/>
       <c r="I234" s="2"/>
@@ -7204,7 +7252,7 @@
       <c r="E235" s="2"/>
       <c r="F235" s="2"/>
       <c r="G235" s="18" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="H235" s="2"/>
       <c r="I235" s="2"/>
@@ -7229,7 +7277,7 @@
       <c r="E236" s="2"/>
       <c r="F236" s="2"/>
       <c r="G236" s="18" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="H236" s="2"/>
       <c r="I236" s="2"/>
@@ -7253,7 +7301,9 @@
       <c r="D237" s="2"/>
       <c r="E237" s="2"/>
       <c r="F237" s="2"/>
-      <c r="G237" s="12"/>
+      <c r="G237" s="18" t="s">
+        <v>163</v>
+      </c>
       <c r="H237" s="2"/>
       <c r="I237" s="2"/>
       <c r="J237" s="2"/>
@@ -7275,10 +7325,8 @@
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
-      <c r="F238" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G238" s="10"/>
+      <c r="F238" s="2"/>
+      <c r="G238" s="12"/>
       <c r="H238" s="2"/>
       <c r="I238" s="2"/>
       <c r="J238" s="2"/>
@@ -7300,10 +7348,10 @@
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
       <c r="E239" s="2"/>
-      <c r="F239" s="2"/>
-      <c r="G239" s="18" t="s">
-        <v>179</v>
-      </c>
+      <c r="F239" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G239" s="10"/>
       <c r="H239" s="2"/>
       <c r="I239" s="2"/>
       <c r="J239" s="2"/>
@@ -7326,7 +7374,9 @@
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
       <c r="F240" s="2"/>
-      <c r="G240" s="18"/>
+      <c r="G240" s="18" t="s">
+        <v>164</v>
+      </c>
       <c r="H240" s="2"/>
       <c r="I240" s="2"/>
       <c r="J240" s="2"/>
@@ -7349,7 +7399,7 @@
       <c r="D241" s="2"/>
       <c r="E241" s="2"/>
       <c r="F241" s="2"/>
-      <c r="G241" s="2"/>
+      <c r="G241" s="18"/>
       <c r="H241" s="2"/>
       <c r="I241" s="2"/>
       <c r="J241" s="2"/>
@@ -7365,24 +7415,14 @@
       <c r="T241" s="2"/>
       <c r="U241" s="2"/>
     </row>
-    <row r="242" spans="1:21" ht="144">
-      <c r="A242" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B242" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C242" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D242" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E242" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F242" s="10"/>
-      <c r="G242" s="8"/>
+    <row r="242" spans="1:21" ht="12">
+      <c r="A242" s="2"/>
+      <c r="B242" s="2"/>
+      <c r="C242" s="2"/>
+      <c r="D242" s="2"/>
+      <c r="E242" s="2"/>
+      <c r="F242" s="2"/>
+      <c r="G242" s="2"/>
       <c r="H242" s="2"/>
       <c r="I242" s="2"/>
       <c r="J242" s="2"/>
@@ -7398,16 +7438,24 @@
       <c r="T242" s="2"/>
       <c r="U242" s="2"/>
     </row>
-    <row r="243" spans="1:21" ht="12">
-      <c r="A243" s="2"/>
-      <c r="B243" s="2"/>
-      <c r="C243" s="2"/>
-      <c r="D243" s="2"/>
-      <c r="E243" s="2"/>
-      <c r="F243" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G243" s="10"/>
+    <row r="243" spans="1:21" ht="144">
+      <c r="A243" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B243" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C243" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D243" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E243" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F243" s="10"/>
+      <c r="G243" s="8"/>
       <c r="H243" s="2"/>
       <c r="I243" s="2"/>
       <c r="J243" s="2"/>
@@ -7429,10 +7477,10 @@
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
       <c r="E244" s="2"/>
-      <c r="F244" s="2"/>
-      <c r="G244" s="18" t="s">
-        <v>180</v>
-      </c>
+      <c r="F244" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G244" s="10"/>
       <c r="H244" s="2"/>
       <c r="I244" s="2"/>
       <c r="J244" s="2"/>
@@ -7456,7 +7504,7 @@
       <c r="E245" s="2"/>
       <c r="F245" s="2"/>
       <c r="G245" s="18" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="H245" s="2"/>
       <c r="I245" s="2"/>
@@ -7481,7 +7529,7 @@
       <c r="E246" s="2"/>
       <c r="F246" s="2"/>
       <c r="G246" s="18" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="H246" s="2"/>
       <c r="I246" s="2"/>
@@ -7506,7 +7554,7 @@
       <c r="E247" s="2"/>
       <c r="F247" s="2"/>
       <c r="G247" s="18" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="H247" s="2"/>
       <c r="I247" s="2"/>
@@ -7530,7 +7578,9 @@
       <c r="D248" s="2"/>
       <c r="E248" s="2"/>
       <c r="F248" s="2"/>
-      <c r="G248" s="18"/>
+      <c r="G248" s="18" t="s">
+        <v>168</v>
+      </c>
       <c r="H248" s="2"/>
       <c r="I248" s="2"/>
       <c r="J248" s="2"/>
@@ -7569,7 +7619,7 @@
       <c r="T249" s="2"/>
       <c r="U249" s="2"/>
     </row>
-    <row r="250" spans="1:21" s="9" customFormat="1" ht="12">
+    <row r="250" spans="1:21" ht="12">
       <c r="A250" s="2"/>
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
@@ -7592,16 +7642,14 @@
       <c r="T250" s="2"/>
       <c r="U250" s="2"/>
     </row>
-    <row r="251" spans="1:21" ht="12">
-      <c r="A251" s="7"/>
-      <c r="B251" s="7"/>
-      <c r="C251" s="7"/>
-      <c r="D251" s="7"/>
-      <c r="E251" s="7"/>
-      <c r="F251" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G251" s="10"/>
+    <row r="251" spans="1:21" s="9" customFormat="1" ht="12">
+      <c r="A251" s="2"/>
+      <c r="B251" s="2"/>
+      <c r="C251" s="2"/>
+      <c r="D251" s="2"/>
+      <c r="E251" s="2"/>
+      <c r="F251" s="2"/>
+      <c r="G251" s="18"/>
       <c r="H251" s="2"/>
       <c r="I251" s="2"/>
       <c r="J251" s="2"/>
@@ -7618,15 +7666,15 @@
       <c r="U251" s="2"/>
     </row>
     <row r="252" spans="1:21" ht="12">
-      <c r="A252" s="2"/>
-      <c r="B252" s="2"/>
-      <c r="C252" s="2"/>
-      <c r="D252" s="2"/>
-      <c r="E252" s="2"/>
-      <c r="F252" s="2"/>
-      <c r="G252" s="18" t="s">
-        <v>184</v>
-      </c>
+      <c r="A252" s="7"/>
+      <c r="B252" s="7"/>
+      <c r="C252" s="7"/>
+      <c r="D252" s="7"/>
+      <c r="E252" s="7"/>
+      <c r="F252" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G252" s="10"/>
       <c r="H252" s="2"/>
       <c r="I252" s="2"/>
       <c r="J252" s="2"/>
@@ -7650,7 +7698,7 @@
       <c r="E253" s="2"/>
       <c r="F253" s="2"/>
       <c r="G253" s="18" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="H253" s="2"/>
       <c r="I253" s="2"/>
@@ -7675,7 +7723,7 @@
       <c r="E254" s="2"/>
       <c r="F254" s="2"/>
       <c r="G254" s="18" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="H254" s="2"/>
       <c r="I254" s="2"/>
@@ -7700,7 +7748,7 @@
       <c r="E255" s="2"/>
       <c r="F255" s="2"/>
       <c r="G255" s="18" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="H255" s="2"/>
       <c r="I255" s="2"/>
@@ -7725,7 +7773,7 @@
       <c r="E256" s="2"/>
       <c r="F256" s="2"/>
       <c r="G256" s="18" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="H256" s="2"/>
       <c r="I256" s="2"/>
@@ -7750,7 +7798,7 @@
       <c r="E257" s="2"/>
       <c r="F257" s="2"/>
       <c r="G257" s="18" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="H257" s="2"/>
       <c r="I257" s="2"/>
@@ -7775,7 +7823,7 @@
       <c r="E258" s="2"/>
       <c r="F258" s="2"/>
       <c r="G258" s="18" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="H258" s="2"/>
       <c r="I258" s="2"/>
@@ -7800,7 +7848,7 @@
       <c r="E259" s="2"/>
       <c r="F259" s="2"/>
       <c r="G259" s="18" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="H259" s="2"/>
       <c r="I259" s="2"/>
@@ -7824,7 +7872,9 @@
       <c r="D260" s="2"/>
       <c r="E260" s="2"/>
       <c r="F260" s="2"/>
-      <c r="G260" s="18"/>
+      <c r="G260" s="18" t="s">
+        <v>176</v>
+      </c>
       <c r="H260" s="2"/>
       <c r="I260" s="2"/>
       <c r="J260" s="2"/>
@@ -7886,7 +7936,7 @@
       <c r="T262" s="2"/>
       <c r="U262" s="2"/>
     </row>
-    <row r="263" spans="1:21" s="9" customFormat="1" ht="12">
+    <row r="263" spans="1:21" ht="12">
       <c r="A263" s="2"/>
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
@@ -7909,16 +7959,14 @@
       <c r="T263" s="2"/>
       <c r="U263" s="2"/>
     </row>
-    <row r="264" spans="1:21" ht="12">
+    <row r="264" spans="1:21" s="9" customFormat="1" ht="12">
       <c r="A264" s="2"/>
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
       <c r="E264" s="2"/>
-      <c r="F264" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G264" s="10"/>
+      <c r="F264" s="2"/>
+      <c r="G264" s="18"/>
       <c r="H264" s="2"/>
       <c r="I264" s="2"/>
       <c r="J264" s="2"/>
@@ -7940,10 +7988,10 @@
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
       <c r="E265" s="2"/>
-      <c r="F265" s="2"/>
-      <c r="G265" s="18" t="s">
-        <v>192</v>
-      </c>
+      <c r="F265" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G265" s="10"/>
       <c r="H265" s="2"/>
       <c r="I265" s="2"/>
       <c r="J265" s="2"/>
@@ -7967,7 +8015,7 @@
       <c r="E266" s="2"/>
       <c r="F266" s="2"/>
       <c r="G266" s="18" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="H266" s="2"/>
       <c r="I266" s="2"/>
@@ -7992,7 +8040,7 @@
       <c r="E267" s="2"/>
       <c r="F267" s="2"/>
       <c r="G267" s="18" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="H267" s="2"/>
       <c r="I267" s="2"/>
@@ -8017,7 +8065,7 @@
       <c r="E268" s="2"/>
       <c r="F268" s="2"/>
       <c r="G268" s="18" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="H268" s="2"/>
       <c r="I268" s="2"/>
@@ -8040,10 +8088,10 @@
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
       <c r="E269" s="2"/>
-      <c r="F269" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="G269" s="10"/>
+      <c r="F269" s="2"/>
+      <c r="G269" s="18" t="s">
+        <v>180</v>
+      </c>
       <c r="H269" s="2"/>
       <c r="I269" s="2"/>
       <c r="J269" s="2"/>
@@ -8065,10 +8113,10 @@
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
       <c r="E270" s="2"/>
-      <c r="F270" s="2"/>
-      <c r="G270" s="18" t="s">
-        <v>196</v>
-      </c>
+      <c r="F270" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G270" s="10"/>
       <c r="H270" s="2"/>
       <c r="I270" s="2"/>
       <c r="J270" s="2"/>
@@ -8092,7 +8140,7 @@
       <c r="E271" s="2"/>
       <c r="F271" s="2"/>
       <c r="G271" s="18" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="H271" s="2"/>
       <c r="I271" s="2"/>
@@ -8117,7 +8165,7 @@
       <c r="E272" s="2"/>
       <c r="F272" s="2"/>
       <c r="G272" s="18" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H272" s="2"/>
       <c r="I272" s="2"/>
@@ -8142,7 +8190,7 @@
       <c r="E273" s="2"/>
       <c r="F273" s="2"/>
       <c r="G273" s="18" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="H273" s="2"/>
       <c r="I273" s="2"/>
@@ -8167,7 +8215,7 @@
       <c r="E274" s="2"/>
       <c r="F274" s="2"/>
       <c r="G274" s="18" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="H274" s="2"/>
       <c r="I274" s="2"/>
@@ -8192,7 +8240,7 @@
       <c r="E275" s="2"/>
       <c r="F275" s="2"/>
       <c r="G275" s="18" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="H275" s="2"/>
       <c r="I275" s="2"/>
@@ -8209,13 +8257,16 @@
       <c r="T275" s="2"/>
       <c r="U275" s="2"/>
     </row>
-    <row r="276" spans="1:21" s="9" customFormat="1" ht="12">
+    <row r="276" spans="1:21" ht="12">
       <c r="A276" s="2"/>
       <c r="B276" s="2"/>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
       <c r="E276" s="2"/>
       <c r="F276" s="2"/>
+      <c r="G276" s="18" t="s">
+        <v>185</v>
+      </c>
       <c r="H276" s="2"/>
       <c r="I276" s="2"/>
       <c r="J276" s="2"/>
@@ -8231,16 +8282,13 @@
       <c r="T276" s="2"/>
       <c r="U276" s="2"/>
     </row>
-    <row r="277" spans="1:21" ht="12">
+    <row r="277" spans="1:21" s="9" customFormat="1" ht="12">
       <c r="A277" s="2"/>
       <c r="B277" s="2"/>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
       <c r="E277" s="2"/>
-      <c r="F277" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="G277" s="10"/>
+      <c r="F277" s="2"/>
       <c r="H277" s="2"/>
       <c r="I277" s="2"/>
       <c r="J277" s="2"/>
@@ -8262,10 +8310,10 @@
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
       <c r="E278" s="2"/>
-      <c r="F278" s="2"/>
-      <c r="G278" s="18" t="s">
-        <v>201</v>
-      </c>
+      <c r="F278" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G278" s="10"/>
       <c r="H278" s="2"/>
       <c r="I278" s="2"/>
       <c r="J278" s="2"/>
@@ -8289,7 +8337,7 @@
       <c r="E279" s="2"/>
       <c r="F279" s="2"/>
       <c r="G279" s="18" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="H279" s="2"/>
       <c r="I279" s="2"/>
@@ -8313,6 +8361,9 @@
       <c r="D280" s="2"/>
       <c r="E280" s="2"/>
       <c r="F280" s="2"/>
+      <c r="G280" s="18" t="s">
+        <v>187</v>
+      </c>
       <c r="H280" s="2"/>
       <c r="I280" s="2"/>
       <c r="J280" s="2"/>
@@ -8334,10 +8385,7 @@
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
       <c r="E281" s="2"/>
-      <c r="F281" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="G281" s="10"/>
+      <c r="F281" s="2"/>
       <c r="H281" s="2"/>
       <c r="I281" s="2"/>
       <c r="J281" s="2"/>
@@ -8359,10 +8407,10 @@
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
       <c r="E282" s="2"/>
-      <c r="F282" s="2"/>
-      <c r="G282" s="18" t="s">
-        <v>203</v>
-      </c>
+      <c r="F282" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G282" s="10"/>
       <c r="H282" s="2"/>
       <c r="I282" s="2"/>
       <c r="J282" s="2"/>
@@ -8386,7 +8434,7 @@
       <c r="E283" s="2"/>
       <c r="F283" s="2"/>
       <c r="G283" s="18" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="H283" s="2"/>
       <c r="I283" s="2"/>
@@ -8411,7 +8459,7 @@
       <c r="E284" s="2"/>
       <c r="F284" s="2"/>
       <c r="G284" s="18" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H284" s="2"/>
       <c r="I284" s="2"/>
@@ -8436,7 +8484,7 @@
       <c r="E285" s="2"/>
       <c r="F285" s="2"/>
       <c r="G285" s="18" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H285" s="2"/>
       <c r="I285" s="2"/>
@@ -8460,6 +8508,9 @@
       <c r="D286" s="2"/>
       <c r="E286" s="2"/>
       <c r="F286" s="2"/>
+      <c r="G286" s="18" t="s">
+        <v>191</v>
+      </c>
       <c r="H286" s="2"/>
       <c r="I286" s="2"/>
       <c r="J286" s="2"/>
@@ -8482,7 +8533,6 @@
       <c r="D287" s="2"/>
       <c r="E287" s="2"/>
       <c r="F287" s="2"/>
-      <c r="G287" s="18"/>
       <c r="H287" s="2"/>
       <c r="I287" s="2"/>
       <c r="J287" s="2"/>
@@ -8505,7 +8555,7 @@
       <c r="D288" s="2"/>
       <c r="E288" s="2"/>
       <c r="F288" s="2"/>
-      <c r="G288" s="12"/>
+      <c r="G288" s="18"/>
       <c r="H288" s="2"/>
       <c r="I288" s="2"/>
       <c r="J288" s="2"/>
@@ -8521,6 +8571,29 @@
       <c r="T288" s="2"/>
       <c r="U288" s="2"/>
     </row>
+    <row r="289" spans="1:21" ht="12">
+      <c r="A289" s="2"/>
+      <c r="B289" s="2"/>
+      <c r="C289" s="2"/>
+      <c r="D289" s="2"/>
+      <c r="E289" s="2"/>
+      <c r="F289" s="2"/>
+      <c r="G289" s="12"/>
+      <c r="H289" s="2"/>
+      <c r="I289" s="2"/>
+      <c r="J289" s="2"/>
+      <c r="K289" s="2"/>
+      <c r="L289" s="2"/>
+      <c r="M289" s="2"/>
+      <c r="N289" s="2"/>
+      <c r="O289" s="2"/>
+      <c r="P289" s="2"/>
+      <c r="Q289" s="2"/>
+      <c r="R289" s="2"/>
+      <c r="S289" s="2"/>
+      <c r="T289" s="2"/>
+      <c r="U289" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Final 1.1 version. Finished after review with Cecile, Hakan, and Todd
</commit_message>
<xml_diff>
--- a/lib/SEMAT_Alpha_Cards_CMU_1.1.xlsx
+++ b/lib/SEMAT_Alpha_Cards_CMU_1.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="20060" yWindow="8580" windowWidth="29520" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="220">
   <si>
     <t>Stakeholders</t>
   </si>
@@ -228,12 +228,6 @@
     <t>Recognized</t>
   </si>
   <si>
-    <t>Stakeholders confirm that system meets their expectations.</t>
-  </si>
-  <si>
-    <t>Software can solve the problem.</t>
-  </si>
-  <si>
     <t>Desired outcomes are clear</t>
   </si>
   <si>
@@ -279,15 +273,9 @@
     <t>Stakeholder representatives confirm system ready for deployment</t>
   </si>
   <si>
-    <t>Software-based solution addresses an identified opportunity</t>
-  </si>
-  <si>
     <t>Problem is clearly articulated</t>
   </si>
   <si>
-    <t>Opportunity addresses problem and stakeholder needs.</t>
-  </si>
-  <si>
     <t>Projected value of software system established</t>
   </si>
   <si>
@@ -303,9 +291,6 @@
     <t>Solution is deployable within constraints</t>
   </si>
   <si>
-    <t>Risks associated with solution are acceptable and manageable.</t>
-  </si>
-  <si>
     <t>Solution demonstrably addresses opportunity</t>
   </si>
   <si>
@@ -342,9 +327,6 @@
     <t>Requirements are prioritized</t>
   </si>
   <si>
-    <t>Rationale and impact are understood</t>
-  </si>
-  <si>
     <t>Requirements are acceptable to stakeholders</t>
   </si>
   <si>
@@ -486,9 +468,6 @@
     <t>A transition plan is defined to adopt new practices and tools</t>
   </si>
   <si>
-    <t>Stakeholders accept external-facing practices &amp; tools</t>
-  </si>
-  <si>
     <t xml:space="preserve">Practices and tools are ready </t>
   </si>
   <si>
@@ -513,9 +492,6 @@
     <t>Team fully embraces principles and values</t>
   </si>
   <si>
-    <t xml:space="preserve">Team captures lessons learned </t>
-  </si>
-  <si>
     <t>Work initiator is known</t>
   </si>
   <si>
@@ -561,9 +537,6 @@
     <t>Progress metrics are identified</t>
   </si>
   <si>
-    <t>Progress is monitored</t>
-  </si>
-  <si>
     <t>Work items are being completed at a steady pace</t>
   </si>
   <si>
@@ -612,9 +585,6 @@
     <t>New requirements are accommodated</t>
   </si>
   <si>
-    <t>Required skills are identified</t>
-  </si>
-  <si>
     <t>Responsibilities and roles are outlined</t>
   </si>
   <si>
@@ -673,13 +643,49 @@
   </si>
   <si>
     <t>Constraints about practices and tools are known</t>
+  </si>
+  <si>
+    <t>Stakeholders accept external-facing practices and tools</t>
+  </si>
+  <si>
+    <t>An idea for a software solution is identified</t>
+  </si>
+  <si>
+    <t>Need for a software solution is confirmed</t>
+  </si>
+  <si>
+    <t>Rationale is understood</t>
+  </si>
+  <si>
+    <t>Impact is understood</t>
+  </si>
+  <si>
+    <t>Non-functional architectural characteristics are considered</t>
+  </si>
+  <si>
+    <t>Required competencies are identifed</t>
+  </si>
+  <si>
+    <t>Stakeholders confirm that system meets their expectations</t>
+  </si>
+  <si>
+    <t>Work context is understood</t>
+  </si>
+  <si>
+    <t>Lessons learned are captured</t>
+  </si>
+  <si>
+    <t>Opportunity addresses problem and stakeholder needs</t>
+  </si>
+  <si>
+    <t>Risks associated with solution are acceptable and manageable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -749,6 +755,12 @@
       <color rgb="FF000000"/>
       <name val="TimesNewRomanPSMT"/>
     </font>
+    <font>
+      <i/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -809,7 +821,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="125">
+  <cellStyleXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -935,8 +947,38 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -994,8 +1036,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="125">
+  <cellStyles count="155">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1058,6 +1103,21 @@
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1120,6 +1180,21 @@
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1507,9 +1582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G216" sqref="G216"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1645,7 +1720,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1670,7 +1745,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1695,7 +1770,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1745,7 +1820,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1770,7 +1845,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="17" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1795,7 +1870,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1820,7 +1895,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="17" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1845,7 +1920,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1895,7 +1970,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1920,7 +1995,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1945,7 +2020,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1995,7 +2070,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -2020,7 +2095,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -2045,7 +2120,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -2070,7 +2145,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -2166,7 +2241,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -2213,7 +2288,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="2"/>
@@ -2239,7 +2314,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -2289,7 +2364,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2" t="s">
-        <v>69</v>
+        <v>215</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2441,7 +2516,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -2466,7 +2541,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -2539,7 +2614,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -2564,7 +2639,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
-        <v>88</v>
+        <v>218</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -2588,8 +2663,8 @@
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="2" t="s">
-        <v>70</v>
+      <c r="G43" s="18" t="s">
+        <v>210</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -2685,7 +2760,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -2710,7 +2785,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -2735,7 +2810,7 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -2760,7 +2835,7 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
@@ -2833,7 +2908,7 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -2858,7 +2933,7 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -2883,7 +2958,7 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2" t="s">
-        <v>94</v>
+        <v>219</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -3002,7 +3077,7 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
@@ -3027,7 +3102,7 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -3052,7 +3127,7 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -3125,7 +3200,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -3150,7 +3225,7 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -3256,7 +3331,7 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="18" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -3281,7 +3356,7 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="18" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
@@ -3377,7 +3452,7 @@
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
@@ -3402,7 +3477,7 @@
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -3427,7 +3502,7 @@
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -3452,7 +3527,7 @@
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="18" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -3477,7 +3552,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="18" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
@@ -3619,7 +3694,7 @@
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="18" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
@@ -3644,7 +3719,7 @@
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
@@ -3669,7 +3744,7 @@
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="18" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
@@ -3694,7 +3769,7 @@
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="18" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -3719,7 +3794,7 @@
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="18" t="s">
-        <v>107</v>
+        <v>211</v>
       </c>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
@@ -3743,7 +3818,9 @@
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
-      <c r="G90" s="18"/>
+      <c r="G90" s="18" t="s">
+        <v>212</v>
+      </c>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
@@ -3861,7 +3938,7 @@
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="18" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
@@ -3886,7 +3963,7 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="18" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
@@ -3911,7 +3988,7 @@
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="18" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
@@ -3936,7 +4013,7 @@
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="18" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
@@ -4009,7 +4086,7 @@
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
       <c r="G101" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
@@ -4034,7 +4111,7 @@
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="18" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
@@ -4130,7 +4207,7 @@
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
       <c r="G106" s="18" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
@@ -4155,7 +4232,7 @@
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
       <c r="G107" s="18" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
@@ -4180,7 +4257,7 @@
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
       <c r="G108" s="18" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
@@ -4285,7 +4362,7 @@
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="18" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
@@ -4310,7 +4387,7 @@
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="18" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
@@ -4335,7 +4412,7 @@
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="18" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
@@ -4360,7 +4437,7 @@
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="18" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
@@ -4385,7 +4462,7 @@
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="18" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
@@ -4410,7 +4487,7 @@
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
       <c r="G117" s="18" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
@@ -4434,7 +4511,9 @@
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
-      <c r="G118" s="12"/>
+      <c r="G118" t="s">
+        <v>213</v>
+      </c>
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
       <c r="J118" s="2"/>
@@ -4483,7 +4562,7 @@
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="18" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
@@ -4508,7 +4587,7 @@
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="18" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
@@ -4533,7 +4612,7 @@
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="18" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
@@ -4652,7 +4731,7 @@
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
       <c r="G127" s="18" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
@@ -4677,7 +4756,7 @@
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="18" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
@@ -4702,7 +4781,7 @@
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="18" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
@@ -4727,7 +4806,7 @@
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
       <c r="G130" s="18" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
@@ -4869,7 +4948,7 @@
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
       <c r="G136" s="18" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H136" s="2"/>
       <c r="I136" s="2"/>
@@ -4894,7 +4973,7 @@
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
       <c r="G137" s="18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
@@ -4990,7 +5069,7 @@
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
       <c r="G141" s="18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H141" s="2"/>
       <c r="I141" s="2"/>
@@ -5015,7 +5094,7 @@
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
       <c r="G142" s="18" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H142" s="2"/>
       <c r="I142" s="2"/>
@@ -5040,7 +5119,7 @@
       <c r="E143" s="2"/>
       <c r="F143" s="2"/>
       <c r="G143" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H143" s="2"/>
       <c r="I143" s="2"/>
@@ -5087,7 +5166,7 @@
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
       <c r="F145" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G145" s="6"/>
       <c r="H145" s="2"/>
@@ -5113,7 +5192,7 @@
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="H146" s="2"/>
       <c r="I146" s="2"/>
@@ -5138,7 +5217,7 @@
       <c r="E147" s="2"/>
       <c r="F147" s="2"/>
       <c r="G147" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H147" s="2"/>
       <c r="I147" s="2"/>
@@ -5163,7 +5242,7 @@
       <c r="E148" s="2"/>
       <c r="F148" s="2"/>
       <c r="G148" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H148" s="2"/>
       <c r="I148" s="2"/>
@@ -5188,7 +5267,7 @@
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H149" s="2"/>
       <c r="I149" s="2"/>
@@ -5213,7 +5292,7 @@
       <c r="E150" s="2"/>
       <c r="F150" s="2"/>
       <c r="G150" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H150" s="2"/>
       <c r="I150" s="2"/>
@@ -5285,7 +5364,7 @@
       <c r="E153" s="2"/>
       <c r="F153" s="2"/>
       <c r="G153" s="18" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H153" s="2"/>
       <c r="I153" s="2"/>
@@ -5459,7 +5538,7 @@
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
       <c r="G160" s="18" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H160" s="2"/>
       <c r="I160" s="2"/>
@@ -5484,7 +5563,7 @@
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
       <c r="G161" s="18" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H161" s="2"/>
       <c r="I161" s="2"/>
@@ -5501,15 +5580,15 @@
       <c r="T161" s="2"/>
       <c r="U161" s="2"/>
     </row>
-    <row r="162" spans="1:21" ht="12">
+    <row r="162" spans="1:21" ht="16">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
-      <c r="G162" s="18" t="s">
-        <v>197</v>
+      <c r="G162" s="19" t="s">
+        <v>214</v>
       </c>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
@@ -5534,7 +5613,7 @@
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
       <c r="G163" s="18" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H163" s="2"/>
       <c r="I163" s="2"/>
@@ -5559,7 +5638,7 @@
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="18" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="H164" s="2"/>
       <c r="I164" s="2"/>
@@ -5584,7 +5663,7 @@
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
       <c r="G165" s="18" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="H165" s="2"/>
       <c r="I165" s="2"/>
@@ -5609,7 +5688,7 @@
       <c r="E166" s="2"/>
       <c r="F166" s="2"/>
       <c r="G166" s="18" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H166" s="2"/>
       <c r="I166" s="2"/>
@@ -5751,7 +5830,7 @@
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
       <c r="G172" s="18" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="H172" s="2"/>
       <c r="I172" s="2"/>
@@ -5776,7 +5855,7 @@
       <c r="E173" s="2"/>
       <c r="F173" s="2"/>
       <c r="G173" s="18" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H173" s="2"/>
       <c r="I173" s="2"/>
@@ -5801,7 +5880,7 @@
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
       <c r="G174" s="18" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H174" s="2"/>
       <c r="I174" s="2"/>
@@ -5826,7 +5905,7 @@
       <c r="E175" s="2"/>
       <c r="F175" s="2"/>
       <c r="G175" s="18" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="H175" s="2"/>
       <c r="I175" s="2"/>
@@ -6014,7 +6093,7 @@
       <c r="E183" s="2"/>
       <c r="F183" s="2"/>
       <c r="G183" s="18" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
@@ -6039,7 +6118,7 @@
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
       <c r="G184" s="18" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="H184" s="2"/>
       <c r="I184" s="2"/>
@@ -6064,7 +6143,7 @@
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
       <c r="G185" s="18" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="H185" s="2"/>
       <c r="I185" s="2"/>
@@ -6089,7 +6168,7 @@
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
       <c r="G186" s="18" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H186" s="2"/>
       <c r="I186" s="2"/>
@@ -6162,7 +6241,7 @@
       <c r="E189" s="2"/>
       <c r="F189" s="2"/>
       <c r="G189" s="18" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H189" s="2"/>
       <c r="I189" s="2"/>
@@ -6187,7 +6266,7 @@
       <c r="E190" s="2"/>
       <c r="F190" s="2"/>
       <c r="G190" s="18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H190" s="2"/>
       <c r="I190" s="2"/>
@@ -6206,7 +6285,7 @@
     </row>
     <row r="191" spans="1:21" ht="12">
       <c r="G191" s="18" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="192" spans="1:21" ht="12">
@@ -6217,7 +6296,7 @@
       <c r="E192" s="2"/>
       <c r="F192" s="2"/>
       <c r="G192" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="H192" s="2"/>
       <c r="I192" s="2"/>
@@ -6242,7 +6321,7 @@
       <c r="E193" s="2"/>
       <c r="F193" s="2"/>
       <c r="G193" s="18" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="H193" s="2"/>
       <c r="I193" s="2"/>
@@ -6361,7 +6440,7 @@
       <c r="E198" s="2"/>
       <c r="F198" s="2"/>
       <c r="G198" s="18" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H198" s="2"/>
       <c r="I198" s="2"/>
@@ -6504,7 +6583,7 @@
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
       <c r="F204" s="15" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="G204" s="10"/>
       <c r="H204" s="2"/>
@@ -6530,7 +6609,7 @@
       <c r="E205" s="2"/>
       <c r="F205" s="2"/>
       <c r="G205" s="18" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="H205" s="2"/>
       <c r="I205" s="2"/>
@@ -6555,7 +6634,7 @@
       <c r="E206" s="2"/>
       <c r="F206" s="2"/>
       <c r="G206" s="18" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="H206" s="2"/>
       <c r="I206" s="2"/>
@@ -6580,7 +6659,7 @@
       <c r="E207" s="2"/>
       <c r="F207" s="2"/>
       <c r="G207" s="18" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="H207" s="2"/>
       <c r="I207" s="2"/>
@@ -6604,7 +6683,9 @@
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
       <c r="F208" s="2"/>
-      <c r="G208" s="18"/>
+      <c r="G208" s="18" t="s">
+        <v>205</v>
+      </c>
       <c r="H208" s="2"/>
       <c r="I208" s="2"/>
       <c r="J208" s="2"/>
@@ -6719,7 +6800,7 @@
       <c r="D213" s="2"/>
       <c r="E213" s="2"/>
       <c r="F213" s="15" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G213" s="10"/>
       <c r="H213" s="2"/>
@@ -6745,7 +6826,7 @@
       <c r="E214" s="2"/>
       <c r="F214" s="2"/>
       <c r="G214" s="18" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="H214" s="2"/>
       <c r="I214" s="2"/>
@@ -6770,7 +6851,7 @@
       <c r="E215" s="2"/>
       <c r="F215" s="2"/>
       <c r="G215" s="18" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H215" s="2"/>
       <c r="I215" s="2"/>
@@ -6795,7 +6876,7 @@
       <c r="E216" s="2"/>
       <c r="F216" s="2"/>
       <c r="G216" s="18" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="H216" s="2"/>
       <c r="I216" s="2"/>
@@ -6820,7 +6901,7 @@
       <c r="E217" s="2"/>
       <c r="F217" s="2"/>
       <c r="G217" s="18" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H217" s="2"/>
       <c r="I217" s="2"/>
@@ -6845,7 +6926,7 @@
       <c r="E218" s="2"/>
       <c r="F218" s="2"/>
       <c r="G218" s="18" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="H218" s="2"/>
       <c r="I218" s="2"/>
@@ -6964,7 +7045,7 @@
       <c r="E223" s="2"/>
       <c r="F223" s="2"/>
       <c r="G223" s="18" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H223" s="2"/>
       <c r="I223" s="2"/>
@@ -6989,7 +7070,7 @@
       <c r="E224" s="2"/>
       <c r="F224" s="2"/>
       <c r="G224" s="18" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H224" s="2"/>
       <c r="I224" s="2"/>
@@ -7014,7 +7095,7 @@
       <c r="E225" s="2"/>
       <c r="F225" s="2"/>
       <c r="G225" s="18" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H225" s="2"/>
       <c r="I225" s="2"/>
@@ -7039,7 +7120,7 @@
       <c r="E226" s="2"/>
       <c r="F226" s="2"/>
       <c r="G226" s="18" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H226" s="2"/>
       <c r="I226" s="2"/>
@@ -7227,7 +7308,7 @@
       <c r="E234" s="2"/>
       <c r="F234" s="2"/>
       <c r="G234" s="18" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="H234" s="2"/>
       <c r="I234" s="2"/>
@@ -7252,7 +7333,7 @@
       <c r="E235" s="2"/>
       <c r="F235" s="2"/>
       <c r="G235" s="18" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="H235" s="2"/>
       <c r="I235" s="2"/>
@@ -7277,7 +7358,7 @@
       <c r="E236" s="2"/>
       <c r="F236" s="2"/>
       <c r="G236" s="18" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H236" s="2"/>
       <c r="I236" s="2"/>
@@ -7302,7 +7383,7 @@
       <c r="E237" s="2"/>
       <c r="F237" s="2"/>
       <c r="G237" s="18" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="H237" s="2"/>
       <c r="I237" s="2"/>
@@ -7348,9 +7429,7 @@
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
       <c r="E239" s="2"/>
-      <c r="F239" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="F239" s="15"/>
       <c r="G239" s="10"/>
       <c r="H239" s="2"/>
       <c r="I239" s="2"/>
@@ -7374,9 +7453,7 @@
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
       <c r="F240" s="2"/>
-      <c r="G240" s="18" t="s">
-        <v>164</v>
-      </c>
+      <c r="G240" s="18"/>
       <c r="H240" s="2"/>
       <c r="I240" s="2"/>
       <c r="J240" s="2"/>
@@ -7504,7 +7581,7 @@
       <c r="E245" s="2"/>
       <c r="F245" s="2"/>
       <c r="G245" s="18" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="H245" s="2"/>
       <c r="I245" s="2"/>
@@ -7529,7 +7606,7 @@
       <c r="E246" s="2"/>
       <c r="F246" s="2"/>
       <c r="G246" s="18" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="H246" s="2"/>
       <c r="I246" s="2"/>
@@ -7554,7 +7631,7 @@
       <c r="E247" s="2"/>
       <c r="F247" s="2"/>
       <c r="G247" s="18" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="H247" s="2"/>
       <c r="I247" s="2"/>
@@ -7579,7 +7656,7 @@
       <c r="E248" s="2"/>
       <c r="F248" s="2"/>
       <c r="G248" s="18" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H248" s="2"/>
       <c r="I248" s="2"/>
@@ -7698,7 +7775,7 @@
       <c r="E253" s="2"/>
       <c r="F253" s="2"/>
       <c r="G253" s="18" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="H253" s="2"/>
       <c r="I253" s="2"/>
@@ -7723,7 +7800,7 @@
       <c r="E254" s="2"/>
       <c r="F254" s="2"/>
       <c r="G254" s="18" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="H254" s="2"/>
       <c r="I254" s="2"/>
@@ -7748,7 +7825,7 @@
       <c r="E255" s="2"/>
       <c r="F255" s="2"/>
       <c r="G255" s="18" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="H255" s="2"/>
       <c r="I255" s="2"/>
@@ -7773,7 +7850,7 @@
       <c r="E256" s="2"/>
       <c r="F256" s="2"/>
       <c r="G256" s="18" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="H256" s="2"/>
       <c r="I256" s="2"/>
@@ -7798,7 +7875,7 @@
       <c r="E257" s="2"/>
       <c r="F257" s="2"/>
       <c r="G257" s="18" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H257" s="2"/>
       <c r="I257" s="2"/>
@@ -7823,7 +7900,7 @@
       <c r="E258" s="2"/>
       <c r="F258" s="2"/>
       <c r="G258" s="18" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H258" s="2"/>
       <c r="I258" s="2"/>
@@ -7848,7 +7925,7 @@
       <c r="E259" s="2"/>
       <c r="F259" s="2"/>
       <c r="G259" s="18" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="H259" s="2"/>
       <c r="I259" s="2"/>
@@ -7873,7 +7950,7 @@
       <c r="E260" s="2"/>
       <c r="F260" s="2"/>
       <c r="G260" s="18" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H260" s="2"/>
       <c r="I260" s="2"/>
@@ -8015,7 +8092,7 @@
       <c r="E266" s="2"/>
       <c r="F266" s="2"/>
       <c r="G266" s="18" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H266" s="2"/>
       <c r="I266" s="2"/>
@@ -8040,7 +8117,7 @@
       <c r="E267" s="2"/>
       <c r="F267" s="2"/>
       <c r="G267" s="18" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="H267" s="2"/>
       <c r="I267" s="2"/>
@@ -8065,7 +8142,7 @@
       <c r="E268" s="2"/>
       <c r="F268" s="2"/>
       <c r="G268" s="18" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H268" s="2"/>
       <c r="I268" s="2"/>
@@ -8089,9 +8166,7 @@
       <c r="D269" s="2"/>
       <c r="E269" s="2"/>
       <c r="F269" s="2"/>
-      <c r="G269" s="18" t="s">
-        <v>180</v>
-      </c>
+      <c r="G269" s="18"/>
       <c r="H269" s="2"/>
       <c r="I269" s="2"/>
       <c r="J269" s="2"/>
@@ -8140,7 +8215,7 @@
       <c r="E271" s="2"/>
       <c r="F271" s="2"/>
       <c r="G271" s="18" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="H271" s="2"/>
       <c r="I271" s="2"/>
@@ -8165,7 +8240,7 @@
       <c r="E272" s="2"/>
       <c r="F272" s="2"/>
       <c r="G272" s="18" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="H272" s="2"/>
       <c r="I272" s="2"/>
@@ -8190,7 +8265,7 @@
       <c r="E273" s="2"/>
       <c r="F273" s="2"/>
       <c r="G273" s="18" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="H273" s="2"/>
       <c r="I273" s="2"/>
@@ -8215,7 +8290,7 @@
       <c r="E274" s="2"/>
       <c r="F274" s="2"/>
       <c r="G274" s="18" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="H274" s="2"/>
       <c r="I274" s="2"/>
@@ -8240,7 +8315,7 @@
       <c r="E275" s="2"/>
       <c r="F275" s="2"/>
       <c r="G275" s="18" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="H275" s="2"/>
       <c r="I275" s="2"/>
@@ -8265,7 +8340,7 @@
       <c r="E276" s="2"/>
       <c r="F276" s="2"/>
       <c r="G276" s="18" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="H276" s="2"/>
       <c r="I276" s="2"/>
@@ -8337,7 +8412,7 @@
       <c r="E279" s="2"/>
       <c r="F279" s="2"/>
       <c r="G279" s="18" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="H279" s="2"/>
       <c r="I279" s="2"/>
@@ -8362,7 +8437,7 @@
       <c r="E280" s="2"/>
       <c r="F280" s="2"/>
       <c r="G280" s="18" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="H280" s="2"/>
       <c r="I280" s="2"/>
@@ -8434,7 +8509,7 @@
       <c r="E283" s="2"/>
       <c r="F283" s="2"/>
       <c r="G283" s="18" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="H283" s="2"/>
       <c r="I283" s="2"/>
@@ -8459,7 +8534,7 @@
       <c r="E284" s="2"/>
       <c r="F284" s="2"/>
       <c r="G284" s="18" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="H284" s="2"/>
       <c r="I284" s="2"/>
@@ -8484,7 +8559,7 @@
       <c r="E285" s="2"/>
       <c r="F285" s="2"/>
       <c r="G285" s="18" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="H285" s="2"/>
       <c r="I285" s="2"/>
@@ -8509,7 +8584,7 @@
       <c r="E286" s="2"/>
       <c r="F286" s="2"/>
       <c r="G286" s="18" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="H286" s="2"/>
       <c r="I286" s="2"/>
@@ -8533,6 +8608,9 @@
       <c r="D287" s="2"/>
       <c r="E287" s="2"/>
       <c r="F287" s="2"/>
+      <c r="G287" s="18" t="s">
+        <v>182</v>
+      </c>
       <c r="H287" s="2"/>
       <c r="I287" s="2"/>
       <c r="J287" s="2"/>
@@ -8578,7 +8656,7 @@
       <c r="D289" s="2"/>
       <c r="E289" s="2"/>
       <c r="F289" s="2"/>
-      <c r="G289" s="12"/>
+      <c r="G289" s="18"/>
       <c r="H289" s="2"/>
       <c r="I289" s="2"/>
       <c r="J289" s="2"/>

</xml_diff>

<commit_message>
Adding in Snapshot History
</commit_message>
<xml_diff>
--- a/lib/SEMAT_Alpha_Cards_CMU_1.1.xlsx
+++ b/lib/SEMAT_Alpha_Cards_CMU_1.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20060" yWindow="8580" windowWidth="29520" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -468,9 +468,6 @@
     <t>A transition plan is defined to adopt new practices and tools</t>
   </si>
   <si>
-    <t xml:space="preserve">Practices and tools are ready </t>
-  </si>
-  <si>
     <t>Team is adopting practices, tools, principles, and values</t>
   </si>
   <si>
@@ -679,6 +676,9 @@
   </si>
   <si>
     <t>Risks associated with solution are acceptable and manageable</t>
+  </si>
+  <si>
+    <t>Key practices and tools are ready</t>
   </si>
 </sst>
 </file>
@@ -1582,9 +1582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G224" sqref="G224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1845,7 +1845,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1895,7 +1895,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2288,7 +2288,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="2"/>
@@ -2314,7 +2314,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -2364,7 +2364,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2516,7 +2516,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -2541,7 +2541,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -2639,7 +2639,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -2664,7 +2664,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -2958,7 +2958,7 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -3527,7 +3527,7 @@
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -3552,7 +3552,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
@@ -3769,7 +3769,7 @@
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -3794,7 +3794,7 @@
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
@@ -3819,7 +3819,7 @@
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
@@ -3963,7 +3963,7 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
@@ -4462,7 +4462,7 @@
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
@@ -4487,7 +4487,7 @@
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
       <c r="G117" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
@@ -4512,7 +4512,7 @@
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
       <c r="G118" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
@@ -4612,7 +4612,7 @@
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
@@ -4756,7 +4756,7 @@
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
@@ -4781,7 +4781,7 @@
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
@@ -5192,7 +5192,7 @@
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H146" s="2"/>
       <c r="I146" s="2"/>
@@ -5588,7 +5588,7 @@
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
       <c r="G162" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
@@ -5663,7 +5663,7 @@
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
       <c r="G165" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H165" s="2"/>
       <c r="I165" s="2"/>
@@ -5830,7 +5830,7 @@
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
       <c r="G172" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H172" s="2"/>
       <c r="I172" s="2"/>
@@ -6583,7 +6583,7 @@
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
       <c r="F204" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G204" s="10"/>
       <c r="H204" s="2"/>
@@ -6609,7 +6609,7 @@
       <c r="E205" s="2"/>
       <c r="F205" s="2"/>
       <c r="G205" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H205" s="2"/>
       <c r="I205" s="2"/>
@@ -6634,7 +6634,7 @@
       <c r="E206" s="2"/>
       <c r="F206" s="2"/>
       <c r="G206" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H206" s="2"/>
       <c r="I206" s="2"/>
@@ -6659,7 +6659,7 @@
       <c r="E207" s="2"/>
       <c r="F207" s="2"/>
       <c r="G207" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H207" s="2"/>
       <c r="I207" s="2"/>
@@ -6684,7 +6684,7 @@
       <c r="E208" s="2"/>
       <c r="F208" s="2"/>
       <c r="G208" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H208" s="2"/>
       <c r="I208" s="2"/>
@@ -6800,7 +6800,7 @@
       <c r="D213" s="2"/>
       <c r="E213" s="2"/>
       <c r="F213" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G213" s="10"/>
       <c r="H213" s="2"/>
@@ -6826,7 +6826,7 @@
       <c r="E214" s="2"/>
       <c r="F214" s="2"/>
       <c r="G214" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H214" s="2"/>
       <c r="I214" s="2"/>
@@ -6876,7 +6876,7 @@
       <c r="E216" s="2"/>
       <c r="F216" s="2"/>
       <c r="G216" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H216" s="2"/>
       <c r="I216" s="2"/>
@@ -6926,7 +6926,7 @@
       <c r="E218" s="2"/>
       <c r="F218" s="2"/>
       <c r="G218" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H218" s="2"/>
       <c r="I218" s="2"/>
@@ -7045,7 +7045,7 @@
       <c r="E223" s="2"/>
       <c r="F223" s="2"/>
       <c r="G223" s="18" t="s">
-        <v>149</v>
+        <v>219</v>
       </c>
       <c r="H223" s="2"/>
       <c r="I223" s="2"/>
@@ -7070,7 +7070,7 @@
       <c r="E224" s="2"/>
       <c r="F224" s="2"/>
       <c r="G224" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H224" s="2"/>
       <c r="I224" s="2"/>
@@ -7095,7 +7095,7 @@
       <c r="E225" s="2"/>
       <c r="F225" s="2"/>
       <c r="G225" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H225" s="2"/>
       <c r="I225" s="2"/>
@@ -7120,7 +7120,7 @@
       <c r="E226" s="2"/>
       <c r="F226" s="2"/>
       <c r="G226" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H226" s="2"/>
       <c r="I226" s="2"/>
@@ -7308,7 +7308,7 @@
       <c r="E234" s="2"/>
       <c r="F234" s="2"/>
       <c r="G234" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H234" s="2"/>
       <c r="I234" s="2"/>
@@ -7333,7 +7333,7 @@
       <c r="E235" s="2"/>
       <c r="F235" s="2"/>
       <c r="G235" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H235" s="2"/>
       <c r="I235" s="2"/>
@@ -7358,7 +7358,7 @@
       <c r="E236" s="2"/>
       <c r="F236" s="2"/>
       <c r="G236" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H236" s="2"/>
       <c r="I236" s="2"/>
@@ -7383,7 +7383,7 @@
       <c r="E237" s="2"/>
       <c r="F237" s="2"/>
       <c r="G237" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H237" s="2"/>
       <c r="I237" s="2"/>
@@ -7581,7 +7581,7 @@
       <c r="E245" s="2"/>
       <c r="F245" s="2"/>
       <c r="G245" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H245" s="2"/>
       <c r="I245" s="2"/>
@@ -7606,7 +7606,7 @@
       <c r="E246" s="2"/>
       <c r="F246" s="2"/>
       <c r="G246" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H246" s="2"/>
       <c r="I246" s="2"/>
@@ -7631,7 +7631,7 @@
       <c r="E247" s="2"/>
       <c r="F247" s="2"/>
       <c r="G247" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H247" s="2"/>
       <c r="I247" s="2"/>
@@ -7656,7 +7656,7 @@
       <c r="E248" s="2"/>
       <c r="F248" s="2"/>
       <c r="G248" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H248" s="2"/>
       <c r="I248" s="2"/>
@@ -7775,7 +7775,7 @@
       <c r="E253" s="2"/>
       <c r="F253" s="2"/>
       <c r="G253" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H253" s="2"/>
       <c r="I253" s="2"/>
@@ -7800,7 +7800,7 @@
       <c r="E254" s="2"/>
       <c r="F254" s="2"/>
       <c r="G254" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H254" s="2"/>
       <c r="I254" s="2"/>
@@ -7825,7 +7825,7 @@
       <c r="E255" s="2"/>
       <c r="F255" s="2"/>
       <c r="G255" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H255" s="2"/>
       <c r="I255" s="2"/>
@@ -7850,7 +7850,7 @@
       <c r="E256" s="2"/>
       <c r="F256" s="2"/>
       <c r="G256" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H256" s="2"/>
       <c r="I256" s="2"/>
@@ -7875,7 +7875,7 @@
       <c r="E257" s="2"/>
       <c r="F257" s="2"/>
       <c r="G257" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H257" s="2"/>
       <c r="I257" s="2"/>
@@ -7900,7 +7900,7 @@
       <c r="E258" s="2"/>
       <c r="F258" s="2"/>
       <c r="G258" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H258" s="2"/>
       <c r="I258" s="2"/>
@@ -7925,7 +7925,7 @@
       <c r="E259" s="2"/>
       <c r="F259" s="2"/>
       <c r="G259" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H259" s="2"/>
       <c r="I259" s="2"/>
@@ -7950,7 +7950,7 @@
       <c r="E260" s="2"/>
       <c r="F260" s="2"/>
       <c r="G260" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H260" s="2"/>
       <c r="I260" s="2"/>
@@ -8092,7 +8092,7 @@
       <c r="E266" s="2"/>
       <c r="F266" s="2"/>
       <c r="G266" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H266" s="2"/>
       <c r="I266" s="2"/>
@@ -8117,7 +8117,7 @@
       <c r="E267" s="2"/>
       <c r="F267" s="2"/>
       <c r="G267" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H267" s="2"/>
       <c r="I267" s="2"/>
@@ -8142,7 +8142,7 @@
       <c r="E268" s="2"/>
       <c r="F268" s="2"/>
       <c r="G268" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H268" s="2"/>
       <c r="I268" s="2"/>
@@ -8215,7 +8215,7 @@
       <c r="E271" s="2"/>
       <c r="F271" s="2"/>
       <c r="G271" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H271" s="2"/>
       <c r="I271" s="2"/>
@@ -8240,7 +8240,7 @@
       <c r="E272" s="2"/>
       <c r="F272" s="2"/>
       <c r="G272" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H272" s="2"/>
       <c r="I272" s="2"/>
@@ -8265,7 +8265,7 @@
       <c r="E273" s="2"/>
       <c r="F273" s="2"/>
       <c r="G273" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H273" s="2"/>
       <c r="I273" s="2"/>
@@ -8290,7 +8290,7 @@
       <c r="E274" s="2"/>
       <c r="F274" s="2"/>
       <c r="G274" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H274" s="2"/>
       <c r="I274" s="2"/>
@@ -8315,7 +8315,7 @@
       <c r="E275" s="2"/>
       <c r="F275" s="2"/>
       <c r="G275" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H275" s="2"/>
       <c r="I275" s="2"/>
@@ -8340,7 +8340,7 @@
       <c r="E276" s="2"/>
       <c r="F276" s="2"/>
       <c r="G276" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H276" s="2"/>
       <c r="I276" s="2"/>
@@ -8412,7 +8412,7 @@
       <c r="E279" s="2"/>
       <c r="F279" s="2"/>
       <c r="G279" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H279" s="2"/>
       <c r="I279" s="2"/>
@@ -8437,7 +8437,7 @@
       <c r="E280" s="2"/>
       <c r="F280" s="2"/>
       <c r="G280" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H280" s="2"/>
       <c r="I280" s="2"/>
@@ -8509,7 +8509,7 @@
       <c r="E283" s="2"/>
       <c r="F283" s="2"/>
       <c r="G283" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H283" s="2"/>
       <c r="I283" s="2"/>
@@ -8534,7 +8534,7 @@
       <c r="E284" s="2"/>
       <c r="F284" s="2"/>
       <c r="G284" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H284" s="2"/>
       <c r="I284" s="2"/>
@@ -8559,7 +8559,7 @@
       <c r="E285" s="2"/>
       <c r="F285" s="2"/>
       <c r="G285" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H285" s="2"/>
       <c r="I285" s="2"/>
@@ -8584,7 +8584,7 @@
       <c r="E286" s="2"/>
       <c r="F286" s="2"/>
       <c r="G286" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H286" s="2"/>
       <c r="I286" s="2"/>
@@ -8609,7 +8609,7 @@
       <c r="E287" s="2"/>
       <c r="F287" s="2"/>
       <c r="G287" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H287" s="2"/>
       <c r="I287" s="2"/>

</xml_diff>